<commit_message>
cleanup and prep for release 1.0
</commit_message>
<xml_diff>
--- a/Scripts/Metal_properties.xlsx
+++ b/Scripts/Metal_properties.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/parham.dehghani/Documents/GitHubl/infrared_tools/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DidomizioMatthew\GitHub\HFITS\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A6706EF-4541-C549-9B7A-968785E0956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D102D457-B026-4C98-B8EC-9B7C4302AD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="15820" xr2:uid="{BDF60127-EB29-3E4E-959D-764F79B14477}"/>
+    <workbookView xWindow="3120" yWindow="0" windowWidth="21600" windowHeight="17550" activeTab="2" xr2:uid="{BDF60127-EB29-3E4E-959D-764F79B14477}"/>
   </bookViews>
   <sheets>
     <sheet name="steel" sheetId="1" r:id="rId1"/>
@@ -7869,16 +7869,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>711200</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>158750</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>330200</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7905,16 +7905,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8096,15 +8096,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>107950</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:colOff>269875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8487,13 +8487,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A61D41D1-3FC1-9346-8311-A7FADF2421FF}">
   <dimension ref="B1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>10</v>
       </c>
@@ -8504,7 +8504,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B2" s="1">
         <v>100</v>
       </c>
@@ -8515,7 +8515,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1">
         <v>200</v>
       </c>
@@ -8526,7 +8526,7 @@
         <v>12.6</v>
       </c>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>300</v>
       </c>
@@ -8537,7 +8537,7 @@
         <v>14.9</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>400</v>
       </c>
@@ -8548,7 +8548,7 @@
         <v>16.600000000000001</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>600</v>
       </c>
@@ -8559,7 +8559,7 @@
         <v>19.8</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>800</v>
       </c>
@@ -8570,7 +8570,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>1000</v>
       </c>
@@ -8581,7 +8581,7 @@
         <v>25.4</v>
       </c>
     </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>1200</v>
       </c>
@@ -8592,7 +8592,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>1500</v>
       </c>
@@ -8617,9 +8617,9 @@
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -8633,7 +8633,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>150</v>
       </c>
@@ -8661,7 +8661,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>200</v>
       </c>
@@ -8675,7 +8675,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>250</v>
       </c>
@@ -8689,7 +8689,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>300</v>
       </c>
@@ -8703,7 +8703,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>400</v>
       </c>
@@ -8717,7 +8717,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>600</v>
       </c>
@@ -8741,13 +8741,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{585B90AB-2FC4-0545-90B2-EEBE0E82E7A3}">
   <dimension ref="B2:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
@@ -8761,7 +8761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
@@ -8775,7 +8775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
         <v>100</v>
       </c>
@@ -8789,7 +8789,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>150</v>
       </c>
@@ -8803,7 +8803,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>200</v>
       </c>
@@ -8817,7 +8817,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>250</v>
       </c>
@@ -8831,7 +8831,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>300</v>
       </c>
@@ -8845,7 +8845,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>400</v>
       </c>
@@ -8859,7 +8859,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>600</v>
       </c>
@@ -8873,7 +8873,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>800</v>
       </c>
@@ -8887,7 +8887,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
         <v>1000</v>
       </c>
@@ -8901,7 +8901,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1">
         <v>1200</v>
       </c>

</xml_diff>